<commit_message>
Encapsulation of Manager objects into Project
+when adding officer to project, add as User object.
+Fixed some formatting to make it prettier
+changed project visiblity logic, allowing only if manager is the project owner
</commit_message>
<xml_diff>
--- a/bto/src/main/data/ProjectList.xlsx
+++ b/bto/src/main/data/ProjectList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\Assignment\2024S2\data_v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/me/Github/sc2002-group-project/bto/src/main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021DB320-1F74-47EA-8228-03A02A2055DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20CCE83-F845-3748-B467-BF1F7B7B3FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="6640" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Project Name</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>Daniel,Emily</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Sleepless Nights</t>
+  </si>
+  <si>
+    <t>Pulau Ubin</t>
   </si>
 </sst>
 </file>
@@ -400,21 +409,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="9" max="10" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" customWidth="1"/>
+    <col min="9" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" customWidth="1"/>
     <col min="13" max="13" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -494,6 +503,44 @@
       </c>
       <c r="M2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>1337</v>
+      </c>
+      <c r="E3">
+        <v>350000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>420</v>
+      </c>
+      <c r="H3">
+        <v>450000</v>
+      </c>
+      <c r="I3" s="1">
+        <v>45703</v>
+      </c>
+      <c r="J3" s="1">
+        <v>45736</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix counting for room type for update flat type in officer
</commit_message>
<xml_diff>
--- a/bto/src/main/data/ProjectList.xlsx
+++ b/bto/src/main/data/ProjectList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/me/Github/sc2002-group-project/bto/src/main/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\sc2002-group-project\bto\src\main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77AA3A2-F75F-E240-9AA2-6E5E1F9B69EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420F6019-7013-4D61-B8B1-26BE2FF2B5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21200" yWindow="-1360" windowWidth="21600" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,18 +430,18 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="9" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" customWidth="1"/>
     <col min="13" max="13" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +482,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -493,7 +493,7 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>350000</v>
@@ -523,7 +523,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -561,7 +561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -599,7 +599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>

</xml_diff>